<commit_message>
More strict validation has been added
</commit_message>
<xml_diff>
--- a/TeamImages/Attributes-Requirements-ver1.xlsx
+++ b/TeamImages/Attributes-Requirements-ver1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sławek\Documents\TeamPolska\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjakubas\git\TeamAssets-master\TeamImages\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="7" xr2:uid="{73D0D82B-5453-4B42-978B-9CFB52DC5A12}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes agreed" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="305">
   <si>
     <t>Grupa</t>
   </si>
@@ -1003,12 +1003,51 @@
   <si>
     <t>validation: non 300DPI validate proportion (3/2) + jpg ONLY</t>
   </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>&lt;product_code&gt;[_&lt;boxoffer&gt;|&lt;offer&gt;|&lt;arr&gt;][_&lt;L&gt;][_&lt;label&gt;][_&lt;xxxDPI&gt;][_&lt;attr1&gt;-&lt;attr2&gt;].&lt;jpg|png&gt;</t>
+  </si>
+  <si>
+    <t>&lt; (less than)</t>
+  </si>
+  <si>
+    <t>&gt; (greater than)</t>
+  </si>
+  <si>
+    <t>: (colon)</t>
+  </si>
+  <si>
+    <t>" (double quote)</t>
+  </si>
+  <si>
+    <t>/ (forward slash)</t>
+  </si>
+  <si>
+    <t>\ (backslash)</t>
+  </si>
+  <si>
+    <t>| (vertical bar or pipe)</t>
+  </si>
+  <si>
+    <t>? (question mark)</t>
+  </si>
+  <si>
+    <t>* (asterisk)</t>
+  </si>
+  <si>
+    <t>CON, PRN, AUX, NUL, COM1, COM2, COM3, COM4, COM5, COM6, COM7, COM8, COM9, LPT1, LPT2, LPT3, LPT4, LPT5, LPT6, LPT7, LPT8, and LPT9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Also avoid these names followed immediately by an extension; for example, NUL.txt is not recommended</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1179,6 +1218,20 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1222,7 +1275,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1290,12 +1343,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Dobry" xfId="2" builtinId="26"/>
-    <cellStyle name="Nagłówek 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Zły" xfId="3" builtinId="27"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1311,9 +1368,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1351,7 +1408,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1457,7 +1514,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1606,7 +1663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5E45CE-9115-4F2E-AD88-08574C7CDC6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
@@ -2499,7 +2556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BA923F-126A-4710-8388-99A4A7F60264}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
@@ -2729,7 +2786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D4F3B-830B-457B-8DC0-AB86063238D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2909,7 +2966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BD2807-63E9-4CC3-A5F3-EBE0F7C6A3D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2921,7 +2978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21DA236-9B53-4B44-8B38-2E374E6A28A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2933,7 +2990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCEDD39-40B3-4CD9-BE9D-B8DB1AAEF087}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2995,7 +3052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E8E587-0438-4D72-BEC6-96DF77A4A77E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3871,10 +3928,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0427C604-CEC1-494C-AC16-5F5600C7564D}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3998,6 +4057,69 @@
         <v>290</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="36" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="36" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="36" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="36" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New scan was run Rules are nor as strict as before Script adds KALORING and SHOTT to possible product code values
</commit_message>
<xml_diff>
--- a/TeamImages/Attributes-Requirements-ver1.xlsx
+++ b/TeamImages/Attributes-Requirements-ver1.xlsx
@@ -1007,9 +1007,6 @@
     <t>template</t>
   </si>
   <si>
-    <t>&lt;product_code&gt;[_&lt;boxoffer&gt;|&lt;offer&gt;|&lt;arr&gt;][_&lt;L&gt;][_&lt;label&gt;][_&lt;xxxDPI&gt;][_&lt;attr1&gt;-&lt;attr2&gt;].&lt;jpg|png&gt;</t>
-  </si>
-  <si>
     <t>&lt; (less than)</t>
   </si>
   <si>
@@ -1041,6 +1038,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Also avoid these names followed immediately by an extension; for example, NUL.txt is not recommended</t>
+  </si>
+  <si>
+    <t>&lt;product_code&gt;[_boxoffer|offer|arr][_L][_label][_&lt;xxx&gt;DPI][_v&lt;xx&gt;][_&lt;attr1&gt;-&lt;attr2&gt;].jpg|png</t>
   </si>
 </sst>
 </file>
@@ -1337,15 +1337,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>151</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="6" t="s">
         <v>190</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="6" t="s">
         <v>197</v>
       </c>
@@ -1794,7 +1794,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="6" t="s">
         <v>189</v>
       </c>
@@ -1815,7 +1815,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="6" t="s">
         <v>193</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="6" t="s">
         <v>194</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="6" t="s">
         <v>195</v>
       </c>
@@ -1880,7 +1880,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="6" t="s">
         <v>196</v>
       </c>
@@ -1901,7 +1901,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="6" t="s">
         <v>198</v>
       </c>
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="26" t="s">
         <v>264</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="31" t="s">
         <v>265</v>
       </c>
@@ -1964,7 +1964,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="27" t="s">
         <v>210</v>
       </c>
@@ -1976,7 +1976,7 @@
       <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="27" t="s">
         <v>252</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="F14" s="27"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="28" t="s">
         <v>259</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
@@ -2028,7 +2028,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="6" t="s">
         <v>20</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="6" t="s">
         <v>188</v>
       </c>
@@ -2067,7 +2067,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>138</v>
       </c>
       <c r="B19" s="29" t="s">
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="29" t="s">
         <v>257</v>
       </c>
@@ -2108,7 +2108,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="29" t="s">
         <v>186</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="29" t="s">
         <v>185</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="29" t="s">
         <v>187</v>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="26" t="s">
         <v>254</v>
       </c>
@@ -2192,7 +2192,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="29" t="s">
         <v>255</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="26" t="s">
         <v>256</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="35" t="s">
         <v>142</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -2257,7 +2257,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="6" t="s">
         <v>201</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="6" t="s">
         <v>202</v>
       </c>
@@ -2299,7 +2299,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+      <c r="A30" s="35"/>
       <c r="C30" s="5" t="s">
         <v>141</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2342,7 +2342,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="35"/>
       <c r="C32" s="9" t="s">
         <v>96</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="35" t="s">
         <v>144</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -2387,7 +2387,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="35"/>
       <c r="C34" s="9" t="s">
         <v>124</v>
       </c>
@@ -2409,7 +2409,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="35"/>
       <c r="C35" s="9" t="s">
         <v>125</v>
       </c>
@@ -2431,7 +2431,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="35" t="s">
         <v>145</v>
       </c>
       <c r="B36" s="24" t="s">
@@ -2457,7 +2457,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="24" t="s">
         <v>260</v>
       </c>
@@ -2483,7 +2483,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="8" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="24" t="s">
         <v>270</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" s="8" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="24" t="s">
         <v>262</v>
       </c>
@@ -2571,11 +2571,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3931,8 +3931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,66 +4058,66 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="33" t="s">
         <v>292</v>
       </c>
       <c r="B17" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="36" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="34" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="34" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="34" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="34" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="34" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="36" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>